<commit_message>
Merged remote base with local project
</commit_message>
<xml_diff>
--- a/public/download/branchnew.xlsx
+++ b/public/download/branchnew.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="109">
   <si>
     <t>LOB</t>
   </si>
@@ -338,19 +338,16 @@
   </si>
   <si>
     <t>powell3@mailsac.com</t>
+  </si>
+  <si>
+    <t>Auditor_Email_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,7 +374,6 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -385,7 +381,6 @@
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -394,136 +389,8 @@
       <name val="Segoe UI"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,194 +403,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -746,249 +427,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -996,63 +438,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1314,61 +710,61 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AX4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="AW1" sqref="AW1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="8.85714285714286" customWidth="1"/>
-    <col min="4" max="4" width="12.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="15.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="10.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="13.7142857142857" customWidth="1"/>
-    <col min="11" max="11" width="17.4285714285714" customWidth="1"/>
-    <col min="12" max="12" width="29.2857142857143" customWidth="1"/>
-    <col min="13" max="13" width="13.8571428571429" customWidth="1"/>
-    <col min="14" max="14" width="19.1428571428571" customWidth="1"/>
-    <col min="15" max="15" width="23.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" customWidth="1"/>
+    <col min="15" max="15" width="23.109375" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="20.4285714285714" customWidth="1"/>
-    <col min="19" max="19" width="25.8571428571429" customWidth="1"/>
-    <col min="20" max="20" width="20.2857142857143" customWidth="1"/>
-    <col min="21" max="21" width="28.5714285714286" customWidth="1"/>
-    <col min="22" max="22" width="32.1428571428571" customWidth="1"/>
-    <col min="23" max="23" width="32.5714285714286" customWidth="1"/>
-    <col min="24" max="24" width="11.4285714285714" customWidth="1"/>
-    <col min="25" max="25" width="12.2857142857143" customWidth="1"/>
-    <col min="32" max="32" width="16.4285714285714" customWidth="1"/>
-    <col min="33" max="33" width="23.4285714285714" customWidth="1"/>
-    <col min="34" max="34" width="22.5714285714286" customWidth="1"/>
-    <col min="35" max="35" width="19.8571428571429" customWidth="1"/>
-    <col min="36" max="36" width="21.2857142857143" customWidth="1"/>
-    <col min="37" max="37" width="12.4285714285714" customWidth="1"/>
+    <col min="17" max="17" width="20.44140625" customWidth="1"/>
+    <col min="19" max="19" width="25.88671875" customWidth="1"/>
+    <col min="20" max="20" width="20.33203125" customWidth="1"/>
+    <col min="21" max="21" width="28.5546875" customWidth="1"/>
+    <col min="22" max="22" width="32.109375" customWidth="1"/>
+    <col min="23" max="23" width="32.5546875" customWidth="1"/>
+    <col min="24" max="24" width="11.44140625" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" customWidth="1"/>
+    <col min="32" max="32" width="16.44140625" customWidth="1"/>
+    <col min="33" max="33" width="23.44140625" customWidth="1"/>
+    <col min="34" max="34" width="22.5546875" customWidth="1"/>
+    <col min="35" max="35" width="19.88671875" customWidth="1"/>
+    <col min="36" max="36" width="21.33203125" customWidth="1"/>
+    <col min="37" max="37" width="12.44140625" customWidth="1"/>
     <col min="38" max="38" width="15" customWidth="1"/>
-    <col min="39" max="39" width="15.7142857142857" customWidth="1"/>
-    <col min="40" max="40" width="19.1428571428571" customWidth="1"/>
-    <col min="41" max="41" width="16.1428571428571" customWidth="1"/>
-    <col min="42" max="42" width="14.1428571428571" customWidth="1"/>
-    <col min="43" max="43" width="13.5714285714286" customWidth="1"/>
-    <col min="44" max="44" width="14.2857142857143" customWidth="1"/>
-    <col min="45" max="45" width="28.1428571428571" customWidth="1"/>
-    <col min="46" max="46" width="23.8571428571429" customWidth="1"/>
-    <col min="47" max="47" width="28.2857142857143" customWidth="1"/>
-    <col min="48" max="48" width="23.5714285714286" customWidth="1"/>
-    <col min="49" max="49" width="25.5714285714286" customWidth="1"/>
-    <col min="50" max="50" width="25.4285714285714" customWidth="1"/>
+    <col min="39" max="39" width="15.6640625" customWidth="1"/>
+    <col min="40" max="40" width="19.109375" customWidth="1"/>
+    <col min="41" max="41" width="16.109375" customWidth="1"/>
+    <col min="42" max="42" width="14.109375" customWidth="1"/>
+    <col min="43" max="43" width="13.5546875" customWidth="1"/>
+    <col min="44" max="44" width="14.33203125" customWidth="1"/>
+    <col min="45" max="45" width="28.109375" customWidth="1"/>
+    <col min="46" max="46" width="23.88671875" customWidth="1"/>
+    <col min="47" max="47" width="28.33203125" customWidth="1"/>
+    <col min="48" max="48" width="23.5546875" customWidth="1"/>
+    <col min="49" max="49" width="25.5546875" customWidth="1"/>
+    <col min="50" max="50" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50">
@@ -1516,10 +912,12 @@
       <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1"/>
+      <c r="AW1" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="AX1" s="1"/>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:50">
       <c r="A2" s="2" t="s">
         <v>48</v>
       </c>
@@ -1626,7 +1024,7 @@
         <v>1234567898</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:36">
+    <row r="3" spans="1:50">
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
@@ -1733,7 +1131,7 @@
         <v>1234567899</v>
       </c>
     </row>
-    <row r="4" ht="16.5" spans="1:36">
+    <row r="4" spans="1:50" ht="16.8">
       <c r="A4" s="2" t="s">
         <v>88</v>
       </c>
@@ -1842,27 +1240,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" display="andrina_hamilton@mailsac.com"/>
-    <hyperlink ref="L3" r:id="rId2" display="hamilton@mailsac.com"/>
-    <hyperlink ref="L4" r:id="rId3" display="hamilton2@mailsac.com"/>
-    <hyperlink ref="P2" r:id="rId4" display="Baker1@mailsac.com" tooltip="mailto:Baker1@mailsac.com"/>
-    <hyperlink ref="P4" r:id="rId5" display="Baker2@mailsac.com"/>
-    <hyperlink ref="P3" r:id="rId6" display="Baker3@mailsac.com"/>
-    <hyperlink ref="S2" r:id="rId7" display="payne@mailsac.com"/>
-    <hyperlink ref="S3" r:id="rId8" display="payne1@mailsac.com"/>
-    <hyperlink ref="S4" r:id="rId9" display="payne2@mailsac.com"/>
-    <hyperlink ref="U2" r:id="rId10" display="taylor@mailsac.com"/>
-    <hyperlink ref="U3" r:id="rId11" display="taylor1@mailsac.com"/>
-    <hyperlink ref="U4" r:id="rId12" display="taylor2@mailsac.com"/>
-    <hyperlink ref="W2" r:id="rId13" display="black1@mailsac.com"/>
-    <hyperlink ref="W3" r:id="rId13" display="black2@mailsac.com"/>
-    <hyperlink ref="W4" r:id="rId13" display="black3@mailsac.com"/>
-    <hyperlink ref="Y2" r:id="rId14" display="powell1@mailsac.com" tooltip="mailto:powell1@mailsac.com"/>
-    <hyperlink ref="Y3" r:id="rId14" display="powell2@mailsac.com" tooltip="mailto:powell1@mailsac.com"/>
-    <hyperlink ref="Y4" r:id="rId14" display="powell3@mailsac.com" tooltip="mailto:powell1@mailsac.com"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="P2" r:id="rId4" tooltip="mailto:Baker1@mailsac.com"/>
+    <hyperlink ref="P4" r:id="rId5"/>
+    <hyperlink ref="P3" r:id="rId6"/>
+    <hyperlink ref="S2" r:id="rId7"/>
+    <hyperlink ref="S3" r:id="rId8"/>
+    <hyperlink ref="S4" r:id="rId9"/>
+    <hyperlink ref="U2" r:id="rId10"/>
+    <hyperlink ref="U3" r:id="rId11"/>
+    <hyperlink ref="U4" r:id="rId12"/>
+    <hyperlink ref="W2" r:id="rId13"/>
+    <hyperlink ref="W3" r:id="rId14"/>
+    <hyperlink ref="W4" r:id="rId15"/>
+    <hyperlink ref="Y2" r:id="rId16" tooltip="mailto:powell1@mailsac.com"/>
+    <hyperlink ref="Y3" r:id="rId17" tooltip="mailto:powell1@mailsac.com"/>
+    <hyperlink ref="Y4" r:id="rId18" tooltip="mailto:powell1@mailsac.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>